<commit_message>
completed periodic table template
</commit_message>
<xml_diff>
--- a/presets/materials/MATERIALS.xlsx
+++ b/presets/materials/MATERIALS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MINECRAFT\dev\Modular Materials 3.0 [1.12.2]\presets\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115776FE-3404-46C1-AE91-4B7DB51654A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E091D51-FFC7-4A58-A974-DAA84B66F669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="122">
   <si>
     <t>Material</t>
   </si>
@@ -303,6 +303,102 @@
   </si>
   <si>
     <t>radon</t>
+  </si>
+  <si>
+    <t>francium</t>
+  </si>
+  <si>
+    <t>radium</t>
+  </si>
+  <si>
+    <t>actinium</t>
+  </si>
+  <si>
+    <t>thorium</t>
+  </si>
+  <si>
+    <t>protactinium</t>
+  </si>
+  <si>
+    <t>uranium</t>
+  </si>
+  <si>
+    <t>neptunium</t>
+  </si>
+  <si>
+    <t>plutonium</t>
+  </si>
+  <si>
+    <t>americium</t>
+  </si>
+  <si>
+    <t>curium</t>
+  </si>
+  <si>
+    <t>berkelium</t>
+  </si>
+  <si>
+    <t>californium</t>
+  </si>
+  <si>
+    <t>einsteinium</t>
+  </si>
+  <si>
+    <t>fermium</t>
+  </si>
+  <si>
+    <t>mendelevium</t>
+  </si>
+  <si>
+    <t>nobelium</t>
+  </si>
+  <si>
+    <t>lawrencium</t>
+  </si>
+  <si>
+    <t>rutherfordium</t>
+  </si>
+  <si>
+    <t>dubnium</t>
+  </si>
+  <si>
+    <t>seaborgium</t>
+  </si>
+  <si>
+    <t>bohrium</t>
+  </si>
+  <si>
+    <t>hassium</t>
+  </si>
+  <si>
+    <t>meitnerium</t>
+  </si>
+  <si>
+    <t>darmstadtium</t>
+  </si>
+  <si>
+    <t>roentgenium</t>
+  </si>
+  <si>
+    <t>copernicium</t>
+  </si>
+  <si>
+    <t>nihonium</t>
+  </si>
+  <si>
+    <t>flerovium</t>
+  </si>
+  <si>
+    <t>moscovium</t>
+  </si>
+  <si>
+    <t>livermorium</t>
+  </si>
+  <si>
+    <t>tennessine</t>
+  </si>
+  <si>
+    <t>oganesson</t>
   </si>
 </sst>
 </file>
@@ -311,7 +407,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -398,7 +494,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -682,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK117"/>
+  <dimension ref="A1:AK149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,11 +790,11 @@
     <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
     <col min="4" max="9" width="9.140625" style="2"/>
-    <col min="10" max="10" width="98.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="2" customWidth="1"/>
     <col min="11" max="30" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -736,14 +832,14 @@
       <c r="AC1" s="8"/>
       <c r="AD1" s="8"/>
     </row>
-    <row r="2" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="5">
-        <v>13</v>
-      </c>
-      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="6"/>
@@ -752,7 +848,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="1"/>
+      <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -774,14 +870,14 @@
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
     </row>
-    <row r="3" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="5">
-        <v>51</v>
-      </c>
-      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="6"/>
@@ -812,14 +908,14 @@
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
     </row>
-    <row r="4" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="5">
-        <v>18</v>
-      </c>
-      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="6"/>
@@ -850,14 +946,14 @@
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
     </row>
-    <row r="5" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="5">
-        <v>33</v>
-      </c>
-      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="6"/>
@@ -888,14 +984,14 @@
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
     </row>
-    <row r="6" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="5">
-        <v>85</v>
-      </c>
-      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="6"/>
@@ -926,14 +1022,14 @@
       <c r="AC6" s="6"/>
       <c r="AD6" s="6"/>
     </row>
-    <row r="7" spans="1:37" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="5">
-        <v>56</v>
-      </c>
-      <c r="C7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="6"/>
@@ -964,204 +1060,247 @@
       <c r="AC7" s="6"/>
       <c r="AD7" s="6"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+    </row>
+    <row r="9" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+    </row>
+    <row r="10" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="11"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="1">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="5">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="G16" s="11"/>
       <c r="J16" s="1"/>
-      <c r="AE16" s="2"/>
-      <c r="AF16" s="2"/>
-      <c r="AG16" s="2"/>
-      <c r="AH16" s="2"/>
-      <c r="AI16" s="2"/>
-      <c r="AJ16" s="2"/>
-      <c r="AK16" s="2"/>
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J17" s="1"/>
-      <c r="AE17" s="2"/>
-      <c r="AF17" s="2"/>
-      <c r="AG17" s="2"/>
-      <c r="AH17" s="2"/>
-      <c r="AI17" s="2"/>
-      <c r="AJ17" s="2"/>
-      <c r="AK17" s="2"/>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J18" s="1"/>
-      <c r="AE18" s="2"/>
-      <c r="AF18" s="2"/>
-      <c r="AG18" s="2"/>
-      <c r="AH18" s="2"/>
-      <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2"/>
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1">
-        <v>27</v>
-      </c>
-      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="5">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J19" s="1"/>
-      <c r="AE19" s="2"/>
-      <c r="AF19" s="2"/>
-      <c r="AG19" s="2"/>
-      <c r="AH19" s="2"/>
-      <c r="AI19" s="2"/>
-      <c r="AJ19" s="2"/>
-      <c r="AK19" s="2"/>
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J20" s="1"/>
-      <c r="AE20" s="2"/>
-      <c r="AF20" s="2"/>
-      <c r="AG20" s="2"/>
-      <c r="AH20" s="2"/>
-      <c r="AI20" s="2"/>
-      <c r="AJ20" s="2"/>
-      <c r="AK20" s="2"/>
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>12</v>
@@ -1177,10 +1316,10 @@
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
@@ -1196,10 +1335,10 @@
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>12</v>
@@ -1215,10 +1354,10 @@
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>12</v>
@@ -1234,10 +1373,10 @@
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>12</v>
@@ -1253,10 +1392,10 @@
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>12</v>
@@ -1272,10 +1411,10 @@
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>12</v>
@@ -1291,10 +1430,10 @@
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>12</v>
@@ -1310,10 +1449,10 @@
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>12</v>
@@ -1329,10 +1468,10 @@
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B30" s="1">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>12</v>
@@ -1348,10 +1487,10 @@
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="B31" s="1">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>12</v>
@@ -1367,10 +1506,10 @@
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="B32" s="1">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>12</v>
@@ -1386,10 +1525,10 @@
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B33" s="1">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>12</v>
@@ -1405,12 +1544,12 @@
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="1">
-        <v>53</v>
-      </c>
-      <c r="C34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="5">
+        <v>33</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J34" s="1"/>
@@ -1424,10 +1563,10 @@
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>12</v>
@@ -1443,10 +1582,10 @@
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B36" s="1">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>12</v>
@@ -1481,10 +1620,10 @@
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>12</v>
@@ -1500,10 +1639,10 @@
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>12</v>
@@ -1519,10 +1658,10 @@
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B40" s="1">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>12</v>
@@ -1538,10 +1677,10 @@
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B41" s="1">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>12</v>
@@ -1557,10 +1696,10 @@
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B42" s="1">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>12</v>
@@ -1576,10 +1715,10 @@
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B43" s="1">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>12</v>
@@ -1595,10 +1734,10 @@
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="B44" s="1">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>12</v>
@@ -1614,10 +1753,10 @@
     </row>
     <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B45" s="1">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>12</v>
@@ -1628,13 +1767,15 @@
       <c r="AG45" s="2"/>
       <c r="AH45" s="2"/>
       <c r="AI45" s="2"/>
+      <c r="AJ45" s="2"/>
+      <c r="AK45" s="2"/>
     </row>
     <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B46" s="1">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>12</v>
@@ -1645,13 +1786,15 @@
       <c r="AG46" s="2"/>
       <c r="AH46" s="2"/>
       <c r="AI46" s="2"/>
+      <c r="AJ46" s="2"/>
+      <c r="AK46" s="2"/>
     </row>
     <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B47" s="1">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>12</v>
@@ -1662,13 +1805,15 @@
       <c r="AG47" s="2"/>
       <c r="AH47" s="2"/>
       <c r="AI47" s="2"/>
+      <c r="AJ47" s="2"/>
+      <c r="AK47" s="2"/>
     </row>
     <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B48" s="1">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>12</v>
@@ -1679,13 +1824,15 @@
       <c r="AG48" s="2"/>
       <c r="AH48" s="2"/>
       <c r="AI48" s="2"/>
-    </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ48" s="2"/>
+      <c r="AK48" s="2"/>
+    </row>
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B49" s="1">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>12</v>
@@ -1696,13 +1843,15 @@
       <c r="AG49" s="2"/>
       <c r="AH49" s="2"/>
       <c r="AI49" s="2"/>
-    </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ49" s="2"/>
+      <c r="AK49" s="2"/>
+    </row>
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="B50" s="1">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>12</v>
@@ -1713,13 +1862,15 @@
       <c r="AG50" s="2"/>
       <c r="AH50" s="2"/>
       <c r="AI50" s="2"/>
-    </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ50" s="2"/>
+      <c r="AK50" s="2"/>
+    </row>
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B51" s="1">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>12</v>
@@ -1730,15 +1881,17 @@
       <c r="AG51" s="2"/>
       <c r="AH51" s="2"/>
       <c r="AI51" s="2"/>
-    </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ51" s="2"/>
+      <c r="AK51" s="2"/>
+    </row>
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" s="1">
-        <v>8</v>
-      </c>
-      <c r="C52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="5">
+        <v>51</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J52" s="1"/>
@@ -1747,13 +1900,15 @@
       <c r="AG52" s="2"/>
       <c r="AH52" s="2"/>
       <c r="AI52" s="2"/>
-    </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ52" s="2"/>
+      <c r="AK52" s="2"/>
+    </row>
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B53" s="1">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>12</v>
@@ -1764,13 +1919,15 @@
       <c r="AG53" s="2"/>
       <c r="AH53" s="2"/>
       <c r="AI53" s="2"/>
-    </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ53" s="2"/>
+      <c r="AK53" s="2"/>
+    </row>
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="B54" s="1">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>12</v>
@@ -1781,13 +1938,15 @@
       <c r="AG54" s="2"/>
       <c r="AH54" s="2"/>
       <c r="AI54" s="2"/>
-    </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ54" s="2"/>
+      <c r="AK54" s="2"/>
+    </row>
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B55" s="1">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>12</v>
@@ -1798,13 +1957,15 @@
       <c r="AG55" s="2"/>
       <c r="AH55" s="2"/>
       <c r="AI55" s="2"/>
-    </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ55" s="2"/>
+      <c r="AK55" s="2"/>
+    </row>
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="B56" s="1">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>12</v>
@@ -1815,15 +1976,17 @@
       <c r="AG56" s="2"/>
       <c r="AH56" s="2"/>
       <c r="AI56" s="2"/>
-    </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ56" s="2"/>
+      <c r="AK56" s="2"/>
+    </row>
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B57" s="1">
-        <v>19</v>
-      </c>
-      <c r="C57" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="5">
+        <v>56</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J57" s="1"/>
@@ -1832,13 +1995,15 @@
       <c r="AG57" s="2"/>
       <c r="AH57" s="2"/>
       <c r="AI57" s="2"/>
-    </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ57" s="2"/>
+      <c r="AK57" s="2"/>
+    </row>
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B58" s="1">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>12</v>
@@ -1849,13 +2014,15 @@
       <c r="AG58" s="2"/>
       <c r="AH58" s="2"/>
       <c r="AI58" s="2"/>
-    </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ58" s="2"/>
+      <c r="AK58" s="2"/>
+    </row>
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B59" s="1">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>12</v>
@@ -1866,13 +2033,15 @@
       <c r="AG59" s="2"/>
       <c r="AH59" s="2"/>
       <c r="AI59" s="2"/>
-    </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ59" s="2"/>
+      <c r="AK59" s="2"/>
+    </row>
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="B60" s="1">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>12</v>
@@ -1883,13 +2052,15 @@
       <c r="AG60" s="2"/>
       <c r="AH60" s="2"/>
       <c r="AI60" s="2"/>
-    </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ60" s="2"/>
+      <c r="AK60" s="2"/>
+    </row>
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B61" s="1">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>12</v>
@@ -1900,13 +2071,15 @@
       <c r="AG61" s="2"/>
       <c r="AH61" s="2"/>
       <c r="AI61" s="2"/>
-    </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ61" s="2"/>
+      <c r="AK61" s="2"/>
+    </row>
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B62" s="1">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>12</v>
@@ -1917,13 +2090,15 @@
       <c r="AG62" s="2"/>
       <c r="AH62" s="2"/>
       <c r="AI62" s="2"/>
-    </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ62" s="2"/>
+      <c r="AK62" s="2"/>
+    </row>
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B63" s="1">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>12</v>
@@ -1935,12 +2110,12 @@
       <c r="AH63" s="2"/>
       <c r="AI63" s="2"/>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="B64" s="1">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>12</v>
@@ -1954,10 +2129,10 @@
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B65" s="1">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>12</v>
@@ -1971,10 +2146,10 @@
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="B66" s="1">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>12</v>
@@ -1988,10 +2163,10 @@
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B67" s="1">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>12</v>
@@ -2005,10 +2180,10 @@
     </row>
     <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="B68" s="1">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>12</v>
@@ -2022,325 +2197,854 @@
     </row>
     <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B69" s="1">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J69" s="1"/>
+      <c r="AE69" s="2"/>
+      <c r="AF69" s="2"/>
+      <c r="AG69" s="2"/>
+      <c r="AH69" s="2"/>
+      <c r="AI69" s="2"/>
     </row>
     <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="B70" s="1">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J70" s="1"/>
+      <c r="AE70" s="2"/>
+      <c r="AF70" s="2"/>
+      <c r="AG70" s="2"/>
+      <c r="AH70" s="2"/>
+      <c r="AI70" s="2"/>
     </row>
     <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="B71" s="1">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J71" s="1"/>
+      <c r="AE71" s="2"/>
+      <c r="AF71" s="2"/>
+      <c r="AG71" s="2"/>
+      <c r="AH71" s="2"/>
+      <c r="AI71" s="2"/>
     </row>
     <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="B72" s="1">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J72" s="1"/>
+      <c r="AE72" s="2"/>
+      <c r="AF72" s="2"/>
+      <c r="AG72" s="2"/>
+      <c r="AH72" s="2"/>
+      <c r="AI72" s="2"/>
     </row>
     <row r="73" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B73" s="1">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J73" s="1"/>
+      <c r="AE73" s="2"/>
+      <c r="AF73" s="2"/>
+      <c r="AG73" s="2"/>
+      <c r="AH73" s="2"/>
+      <c r="AI73" s="2"/>
     </row>
     <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="B74" s="1">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J74" s="1"/>
+      <c r="AE74" s="2"/>
+      <c r="AF74" s="2"/>
+      <c r="AG74" s="2"/>
+      <c r="AH74" s="2"/>
+      <c r="AI74" s="2"/>
     </row>
     <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="B75" s="1">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J75" s="1"/>
+      <c r="AE75" s="2"/>
+      <c r="AF75" s="2"/>
+      <c r="AG75" s="2"/>
+      <c r="AH75" s="2"/>
+      <c r="AI75" s="2"/>
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B76" s="1">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J76" s="1"/>
+      <c r="AE76" s="2"/>
+      <c r="AF76" s="2"/>
+      <c r="AG76" s="2"/>
+      <c r="AH76" s="2"/>
+      <c r="AI76" s="2"/>
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B77" s="1">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J77" s="1"/>
+      <c r="AE77" s="2"/>
+      <c r="AF77" s="2"/>
+      <c r="AG77" s="2"/>
+      <c r="AH77" s="2"/>
+      <c r="AI77" s="2"/>
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B78" s="1">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J78" s="1"/>
+      <c r="AE78" s="2"/>
+      <c r="AF78" s="2"/>
+      <c r="AG78" s="2"/>
+      <c r="AH78" s="2"/>
+      <c r="AI78" s="2"/>
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="B79" s="1">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J79" s="1"/>
+      <c r="AE79" s="2"/>
+      <c r="AF79" s="2"/>
+      <c r="AG79" s="2"/>
+      <c r="AH79" s="2"/>
+      <c r="AI79" s="2"/>
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="B80" s="1">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J80" s="1"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE80" s="2"/>
+      <c r="AF80" s="2"/>
+      <c r="AG80" s="2"/>
+      <c r="AH80" s="2"/>
+      <c r="AI80" s="2"/>
+    </row>
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B81" s="1">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J81" s="1"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE81" s="2"/>
+      <c r="AF81" s="2"/>
+      <c r="AG81" s="2"/>
+      <c r="AH81" s="2"/>
+      <c r="AI81" s="2"/>
+    </row>
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="B82" s="1">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J82" s="1"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE82" s="2"/>
+      <c r="AF82" s="2"/>
+      <c r="AG82" s="2"/>
+      <c r="AH82" s="2"/>
+      <c r="AI82" s="2"/>
+    </row>
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="B83" s="1">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J83" s="1"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE83" s="2"/>
+      <c r="AF83" s="2"/>
+      <c r="AG83" s="2"/>
+      <c r="AH83" s="2"/>
+      <c r="AI83" s="2"/>
+    </row>
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B84" s="1">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J84" s="1"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE84" s="2"/>
+      <c r="AF84" s="2"/>
+      <c r="AG84" s="2"/>
+      <c r="AH84" s="2"/>
+      <c r="AI84" s="2"/>
+    </row>
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="B85" s="1">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J85" s="1"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE85" s="2"/>
+      <c r="AF85" s="2"/>
+      <c r="AG85" s="2"/>
+      <c r="AH85" s="2"/>
+      <c r="AI85" s="2"/>
+    </row>
+    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B86" s="1">
-        <v>30</v>
-      </c>
-      <c r="C86" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" s="5">
+        <v>85</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J86" s="1"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE86" s="2"/>
+      <c r="AF86" s="2"/>
+      <c r="AG86" s="2"/>
+      <c r="AH86" s="2"/>
+      <c r="AI86" s="2"/>
+    </row>
+    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="B87" s="1">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J87" s="1"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE87" s="2"/>
+      <c r="AF87" s="2"/>
+      <c r="AG87" s="2"/>
+      <c r="AH87" s="2"/>
+      <c r="AI87" s="2"/>
+    </row>
+    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A88" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B88" s="1">
+        <v>87</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J88" s="1"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE88" s="2"/>
+      <c r="AF88" s="2"/>
+      <c r="AG88" s="2"/>
+      <c r="AH88" s="2"/>
+      <c r="AI88" s="2"/>
+    </row>
+    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A89" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" s="1">
+        <v>88</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J89" s="1"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE89" s="2"/>
+      <c r="AF89" s="2"/>
+      <c r="AG89" s="2"/>
+      <c r="AH89" s="2"/>
+      <c r="AI89" s="2"/>
+    </row>
+    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A90" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90" s="5">
+        <v>89</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="J90" s="1"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE90" s="2"/>
+      <c r="AF90" s="2"/>
+      <c r="AG90" s="2"/>
+      <c r="AH90" s="2"/>
+      <c r="AI90" s="2"/>
+    </row>
+    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B91" s="1">
+        <v>90</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J91" s="1"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE91" s="2"/>
+      <c r="AF91" s="2"/>
+      <c r="AG91" s="2"/>
+      <c r="AH91" s="2"/>
+      <c r="AI91" s="2"/>
+    </row>
+    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B92" s="1">
+        <v>91</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J92" s="1"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE92" s="2"/>
+      <c r="AF92" s="2"/>
+      <c r="AG92" s="2"/>
+      <c r="AH92" s="2"/>
+      <c r="AI92" s="2"/>
+    </row>
+    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93" s="1">
+        <v>92</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J93" s="1"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE93" s="2"/>
+      <c r="AF93" s="2"/>
+      <c r="AG93" s="2"/>
+      <c r="AH93" s="2"/>
+      <c r="AI93" s="2"/>
+    </row>
+    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B94" s="1">
+        <v>93</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J94" s="1"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE94" s="2"/>
+      <c r="AF94" s="2"/>
+      <c r="AG94" s="2"/>
+      <c r="AH94" s="2"/>
+      <c r="AI94" s="2"/>
+    </row>
+    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A95" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B95" s="1">
+        <v>94</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J95" s="1"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="AE95" s="2"/>
+      <c r="AF95" s="2"/>
+      <c r="AG95" s="2"/>
+      <c r="AH95" s="2"/>
+      <c r="AI95" s="2"/>
+    </row>
+    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A96" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B96" s="5">
+        <v>95</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="J96" s="1"/>
-    </row>
-    <row r="97" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="AE96" s="2"/>
+      <c r="AF96" s="2"/>
+      <c r="AG96" s="2"/>
+      <c r="AH96" s="2"/>
+      <c r="AI96" s="2"/>
+    </row>
+    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A97" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97" s="1">
+        <v>96</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J97" s="1"/>
-    </row>
-    <row r="98" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="AE97" s="2"/>
+      <c r="AF97" s="2"/>
+      <c r="AG97" s="2"/>
+      <c r="AH97" s="2"/>
+      <c r="AI97" s="2"/>
+    </row>
+    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" s="5">
+        <v>97</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="J98" s="1"/>
     </row>
-    <row r="99" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A99" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" s="1">
+        <v>98</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J99" s="1"/>
     </row>
-    <row r="100" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A100" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" s="1">
+        <v>99</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J100" s="1"/>
     </row>
-    <row r="101" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A101" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B101" s="1">
+        <v>100</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J101" s="1"/>
     </row>
-    <row r="102" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B102" s="1">
+        <v>101</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J102" s="1"/>
     </row>
-    <row r="103" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A103" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B103" s="1">
+        <v>102</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J103" s="1"/>
     </row>
-    <row r="104" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J104" s="12"/>
-    </row>
-    <row r="105" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J105" s="12"/>
-    </row>
-    <row r="106" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J106" s="12"/>
-    </row>
-    <row r="107" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J107" s="12"/>
-    </row>
-    <row r="108" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J108" s="12"/>
-    </row>
-    <row r="109" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J109" s="12"/>
-    </row>
-    <row r="110" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J110" s="12"/>
-    </row>
-    <row r="111" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J111" s="12"/>
-    </row>
-    <row r="112" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J112" s="12"/>
-    </row>
-    <row r="113" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J113" s="12"/>
-    </row>
-    <row r="114" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J114" s="12"/>
-    </row>
-    <row r="115" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J115" s="12"/>
-    </row>
-    <row r="116" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J116" s="12"/>
-    </row>
-    <row r="117" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J117" s="12"/>
+    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A104" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B104" s="1">
+        <v>103</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J104" s="1"/>
+    </row>
+    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A105" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105" s="1">
+        <v>104</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J105" s="1"/>
+    </row>
+    <row r="106" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A106" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" s="1">
+        <v>105</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J106" s="1"/>
+    </row>
+    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A107" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" s="1">
+        <v>106</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J107" s="1"/>
+    </row>
+    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A108" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B108" s="1">
+        <v>107</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J108" s="1"/>
+    </row>
+    <row r="109" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A109" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B109" s="1">
+        <v>108</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J109" s="1"/>
+    </row>
+    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A110" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" s="1">
+        <v>109</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J110" s="1"/>
+    </row>
+    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A111" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" s="1">
+        <v>110</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J111" s="1"/>
+    </row>
+    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A112" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B112" s="1">
+        <v>111</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J112" s="1"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B113" s="1">
+        <v>112</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J113" s="1"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B114" s="1">
+        <v>113</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J114" s="1"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B115" s="1">
+        <v>114</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J115" s="1"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B116" s="1">
+        <v>115</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J116" s="1"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B117" s="1">
+        <v>116</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J117" s="1"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B118" s="1">
+        <v>117</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J118" s="1"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B119" s="1">
+        <v>118</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J119" s="1"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J120" s="1"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J121" s="1"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J122" s="1"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J123" s="1"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J124" s="1"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J125" s="1"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J126" s="1"/>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J127" s="1"/>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J128" s="1"/>
+    </row>
+    <row r="129" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J129" s="1"/>
+    </row>
+    <row r="130" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J130" s="1"/>
+    </row>
+    <row r="131" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J131" s="1"/>
+    </row>
+    <row r="132" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J132" s="1"/>
+    </row>
+    <row r="133" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J133" s="1"/>
+    </row>
+    <row r="134" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J134" s="1"/>
+    </row>
+    <row r="135" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J135" s="1"/>
+    </row>
+    <row r="136" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J136" s="12"/>
+    </row>
+    <row r="137" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J137" s="12"/>
+    </row>
+    <row r="138" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J138" s="12"/>
+    </row>
+    <row r="139" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J139" s="12"/>
+    </row>
+    <row r="140" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J140" s="12"/>
+    </row>
+    <row r="141" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J141" s="12"/>
+    </row>
+    <row r="142" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J142" s="12"/>
+    </row>
+    <row r="143" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J143" s="12"/>
+    </row>
+    <row r="144" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J144" s="12"/>
+    </row>
+    <row r="145" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J145" s="12"/>
+    </row>
+    <row r="146" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J146" s="12"/>
+    </row>
+    <row r="147" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J147" s="12"/>
+    </row>
+    <row r="148" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J148" s="12"/>
+    </row>
+    <row r="149" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J149" s="12"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B87">
-    <sortCondition ref="A1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C119">
+    <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>